<commit_message>
Ajout des nouvelles instances
</commit_message>
<xml_diff>
--- a/src/ressources/coutOptimalParInstance.xlsx
+++ b/src/ressources/coutOptimalParInstance.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdelobelle/Documents/enseignements/paris/2025-2026/s1/PAA/projet/instance/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdelobelle/Documents/enseignements/paris/2025-2026/s1/PAA/projet/instances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45839DAD-4E0C-DA4B-9825-F5B76646F129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C15C57-01DB-D84A-B9CB-9E5856CC91A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16360" xr2:uid="{D15D0B4D-8D42-C74A-86C1-64A36FE8CB57}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>nom fichier</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>instance6</t>
+  </si>
+  <si>
+    <t>instance7</t>
   </si>
 </sst>
 </file>
@@ -129,7 +132,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -451,7 +454,7 @@
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -480,7 +483,7 @@
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3">
         <v>0.95039682539682502</v>
       </c>
     </row>
@@ -505,7 +508,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="5">
-        <v>23.919019035692099</v>
+        <v>12.504761904761899</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -513,12 +516,16 @@
         <v>7</v>
       </c>
       <c r="B7" s="5">
-        <v>17.8767949002387</v>
+        <v>1.2523809523809499</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4">
+        <v>49.884303350970001</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>

</xml_diff>

<commit_message>
ajout d'un main pour lancer le projet, ajout d'un launch.json pour simuler la ligne de commande, modification des menus, optimisation du chargement de fichier, de la sauvegarde de solution et du lancement de l'algorithme
</commit_message>
<xml_diff>
--- a/src/ressources/coutOptimalParInstance.xlsx
+++ b/src/ressources/coutOptimalParInstance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annel\Documents\Licence\L3\PAA\Projet\PROJET_PAA\src\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007690D9-6841-4927-A88B-6BD57F1533B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75249673-6886-4E89-8DBF-8CFA77B9DDC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D15D0B4D-8D42-C74A-86C1-64A36FE8CB57}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>nom fichier</t>
   </si>
@@ -69,9 +69,6 @@
     <t>2.0873015873015874</t>
   </si>
   <si>
-    <t>3.284656084656085</t>
-  </si>
-  <si>
     <t>2.1660714285714286</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>Cout algo2</t>
+  </si>
+  <si>
+    <t>maison manquante 3.284656084656085</t>
   </si>
 </sst>
 </file>
@@ -116,7 +116,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -139,17 +139,78 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -466,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F055162F-0EB5-E149-B0A3-18A189CD2A51}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -477,9 +538,10 @@
     <col min="1" max="1" width="26.1640625" customWidth="1"/>
     <col min="2" max="2" width="34.33203125" customWidth="1"/>
     <col min="3" max="3" width="35.9140625" customWidth="1"/>
+    <col min="4" max="4" width="28.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -487,115 +549,141 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="8">
         <v>0.48412698412698402</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" s="4">
+        <v>0.69841269841269804</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="6">
         <v>0.95039682539682502</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3" s="4">
+        <v>1.0595238095238</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="8">
         <v>0</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="8">
         <v>0</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="8">
         <v>12.504761904761899</v>
       </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1.5119047619047601</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="8">
         <v>1.2523809523809499</v>
       </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.75595238095238004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="7">
         <v>49.884303350970001</v>
       </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="4">
+        <v>5.0941798941798897</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B9" s="5"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
     </row>

</xml_diff>

<commit_message>
Modification README, correction des accents dans tout le programme, ajout des fichiers .ddl en cas d'erreur avec javaFX, passage de javaFX 25 à javaFX 21
</commit_message>
<xml_diff>
--- a/src/ressources/coutOptimalParInstance.xlsx
+++ b/src/ressources/coutOptimalParInstance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annel\Documents\Licence\L3\PAA\Projet\PROJET_PAA\src\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6539C2-9EBE-43A6-B1FE-9ABDD231EEAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B3F777-E2C9-4F8B-88DA-517C918E945C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D15D0B4D-8D42-C74A-86C1-64A36FE8CB57}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>nom fichier</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>0.6984126984126984</t>
+  </si>
+  <si>
+    <t>5.094179894179893</t>
   </si>
 </sst>
 </file>
@@ -143,7 +146,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -166,75 +169,17 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -551,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F055162F-0EB5-E149-B0A3-18A189CD2A51}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -566,62 +511,53 @@
     <col min="5" max="5" width="33.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7">
-        <v>0.48412698412698402</v>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D2" s="3">
         <v>0.69841269841269804</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5">
-        <v>0.95039682539682502</v>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D3" s="3">
         <v>1.0595238095238</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="3">
         <v>0</v>
       </c>
       <c r="C4" s="3">
@@ -630,15 +566,12 @@
       <c r="D4" s="3">
         <v>0</v>
       </c>
-      <c r="E4" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="3">
         <v>0</v>
       </c>
       <c r="C5" s="3">
@@ -647,174 +580,68 @@
       <c r="D5" s="3">
         <v>0</v>
       </c>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="7">
-        <v>12.504761904761899</v>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D6" s="3">
         <v>1.5119047619047601</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="7">
-        <v>1.2523809523809499</v>
+      <c r="B7" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D7" s="3">
         <v>0.75595238095238004</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="6">
-        <v>49.884303350970001</v>
+      <c r="B8" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D8" s="3">
         <v>5.0941798941798897</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="D9" s="3"/>
-      <c r="E9" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="C10" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>